<commit_message>
Added New JSON Files
</commit_message>
<xml_diff>
--- a/data analysis/User Stats and History/Top_Reviewers_Analysis.xlsx
+++ b/data analysis/User Stats and History/Top_Reviewers_Analysis.xlsx
@@ -1103,22 +1103,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="9" width="46.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" customWidth="1"/>
+    <col min="6" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1737,7 +1738,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>71</v>
       </c>

</xml_diff>